<commit_message>
Case and Fatality Demographics Data Updated
</commit_message>
<xml_diff>
--- a/CaseAndFatalityDemographicsData/2021-01-29.xlsx
+++ b/CaseAndFatalityDemographicsData/2021-01-29.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdavis197\Desktop\Leadership Reports\Demographics Thursday\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61075A07-7360-4E0F-AE8F-0A192C3B4190}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E4C632F-6349-4FAE-B49E-EF2EABED02BA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="806" firstSheet="2" activeTab="4" xr2:uid="{A6E7ED99-6879-4496-BF23-313330724014}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="806" xr2:uid="{A6E7ED99-6879-4496-BF23-313330724014}"/>
   </bookViews>
   <sheets>
     <sheet name="Cases by Age Group" sheetId="3" r:id="rId1"/>
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBBE98AD-F551-4399-A212-2161860B6EB7}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -573,11 +573,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C2" s="12">
         <f>B2/$B$15</f>
-        <v>3.6545710914793819E-3</v>
+        <v>3.615687831438051E-3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -585,11 +585,11 @@
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <v>1228</v>
+        <v>1234</v>
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C15" si="0">B3/$B$15</f>
-        <v>1.7668556300538114E-2</v>
+        <v>1.7497093270566883E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -597,11 +597,11 @@
         <v>4</v>
       </c>
       <c r="B4" s="4">
-        <v>3262</v>
+        <v>3294</v>
       </c>
       <c r="C4" s="12">
         <f t="shared" si="0"/>
-        <v>4.6933901182699779E-2</v>
+        <v>4.6706179281399765E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -609,11 +609,11 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>13819</v>
+        <v>14024</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" si="0"/>
-        <v>0.19882881068170699</v>
+        <v>0.19884865156112638</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -621,11 +621,11 @@
         <v>6</v>
       </c>
       <c r="B6" s="4">
-        <v>15064</v>
+        <v>15348</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" si="0"/>
-        <v>0.21674196426002129</v>
+        <v>0.21762186994867141</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -633,11 +633,11 @@
         <v>7</v>
       </c>
       <c r="B7" s="4">
-        <v>13263</v>
+        <v>13492</v>
       </c>
       <c r="C7" s="12">
         <f t="shared" si="0"/>
-        <v>0.1908290408909096</v>
+        <v>0.19130533420298898</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -645,11 +645,11 @@
         <v>8</v>
       </c>
       <c r="B8" s="4">
-        <v>11292</v>
+        <v>11467</v>
       </c>
       <c r="C8" s="12">
         <f t="shared" si="0"/>
-        <v>0.16247014474403615</v>
+        <v>0.16259251907098091</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -657,11 +657,11 @@
         <v>9</v>
       </c>
       <c r="B9" s="4">
-        <v>4125</v>
+        <v>4163</v>
       </c>
       <c r="C9" s="12">
         <f t="shared" si="0"/>
-        <v>5.9350810048631693E-2</v>
+        <v>5.902787624422199E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -669,11 +669,11 @@
         <v>10</v>
       </c>
       <c r="B10" s="4">
-        <v>2776</v>
+        <v>2805</v>
       </c>
       <c r="C10" s="12">
         <f t="shared" si="0"/>
-        <v>3.9941296653333715E-2</v>
+        <v>3.9772566145818561E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -681,11 +681,11 @@
         <v>11</v>
       </c>
       <c r="B11" s="4">
-        <v>1656</v>
+        <v>1669</v>
       </c>
       <c r="C11" s="12">
         <f t="shared" si="0"/>
-        <v>2.3826652470432506E-2</v>
+        <v>2.3665031335961206E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -693,11 +693,11 @@
         <v>12</v>
       </c>
       <c r="B12" s="4">
-        <v>1074</v>
+        <v>1082</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" si="0"/>
-        <v>1.5452792725389198E-2</v>
+        <v>1.5341859739670477E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -705,11 +705,11 @@
         <v>13</v>
       </c>
       <c r="B13" s="4">
-        <v>1675</v>
+        <v>1679</v>
       </c>
       <c r="C13" s="12">
         <f t="shared" si="0"/>
-        <v>2.4100025898535295E-2</v>
+        <v>2.3806823015625443E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -721,7 +721,7 @@
       </c>
       <c r="C14" s="12">
         <f t="shared" si="0"/>
-        <v>2.0143305228626516E-4</v>
+        <v>1.9850835152993222E-4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -730,7 +730,7 @@
       </c>
       <c r="B15" s="1">
         <f>SUM(B2:B14)</f>
-        <v>69502</v>
+        <v>70526</v>
       </c>
       <c r="C15" s="11">
         <f t="shared" si="0"/>
@@ -747,7 +747,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -768,11 +768,11 @@
         <v>16</v>
       </c>
       <c r="B2" s="4">
-        <v>23935</v>
+        <v>24069</v>
       </c>
       <c r="C2" s="12">
         <f>B2/$B$5</f>
-        <v>0.3443785790336969</v>
+        <v>0.34127839378385277</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -780,11 +780,11 @@
         <v>17</v>
       </c>
       <c r="B3" s="4">
-        <v>44684</v>
+        <v>45567</v>
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C5" si="0">B3/$B$5</f>
-        <v>0.64291675059710507</v>
+        <v>0.64610214672603017</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -792,11 +792,11 @@
         <v>18</v>
       </c>
       <c r="B4" s="4">
-        <v>883</v>
+        <v>890</v>
       </c>
       <c r="C4" s="12">
         <f t="shared" si="0"/>
-        <v>1.2704670369198008E-2</v>
+        <v>1.261945949011712E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -805,7 +805,7 @@
       </c>
       <c r="B5" s="1">
         <f>SUM(B2:B4)</f>
-        <v>69502</v>
+        <v>70526</v>
       </c>
       <c r="C5" s="11">
         <f t="shared" si="0"/>
@@ -822,7 +822,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -846,11 +846,11 @@
         <v>23</v>
       </c>
       <c r="B2" s="4">
-        <v>914</v>
+        <v>920</v>
       </c>
       <c r="C2" s="12">
         <f>B2/$B$8</f>
-        <v>1.3150700699260453E-2</v>
+        <v>1.3044834529109832E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -858,11 +858,11 @@
         <v>21</v>
       </c>
       <c r="B3" s="4">
-        <v>11474</v>
+        <v>11750</v>
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C8" si="0">B3/$B$8</f>
-        <v>0.16508877442375758</v>
+        <v>0.16660522360547883</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -870,11 +870,11 @@
         <v>22</v>
       </c>
       <c r="B4" s="4">
-        <v>26718</v>
+        <v>26927</v>
       </c>
       <c r="C4" s="12">
         <f t="shared" si="0"/>
-        <v>0.38442059221317371</v>
+        <v>0.38180245583189176</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -882,11 +882,11 @@
         <v>25</v>
       </c>
       <c r="B5" s="4">
-        <v>353</v>
+        <v>365</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" si="0"/>
-        <v>5.0789905326465426E-3</v>
+        <v>5.1753963077446619E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -894,11 +894,11 @@
         <v>20</v>
       </c>
       <c r="B6" s="4">
-        <v>21947</v>
+        <v>22453</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" si="0"/>
-        <v>0.31577508560904721</v>
+        <v>0.31836485835011202</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -906,11 +906,11 @@
         <v>18</v>
       </c>
       <c r="B7" s="4">
-        <v>8096</v>
+        <v>8111</v>
       </c>
       <c r="C7" s="12">
         <f t="shared" si="0"/>
-        <v>0.11648585652211448</v>
+        <v>0.11500723137566288</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -919,7 +919,7 @@
       </c>
       <c r="B8" s="1">
         <f>SUM(B2:B7)</f>
-        <v>69502</v>
+        <v>70526</v>
       </c>
       <c r="C8" s="11">
         <f t="shared" si="0"/>
@@ -936,7 +936,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -964,7 +964,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/$B$15</f>
-        <v>1.4833714065327677E-4</v>
+        <v>1.3893520062242969E-4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -976,7 +976,7 @@
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C15" si="0">B3/$B$15</f>
-        <v>2.3733942504524283E-4</v>
+        <v>2.222963209958875E-4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -984,11 +984,11 @@
         <v>4</v>
       </c>
       <c r="B4" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" s="12">
         <f t="shared" si="0"/>
-        <v>7.1201827513572846E-4</v>
+        <v>6.9467600311214853E-4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -996,11 +996,11 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" si="0"/>
-        <v>4.9841279259500992E-3</v>
+        <v>4.8627320217850397E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1008,11 +1008,11 @@
         <v>6</v>
       </c>
       <c r="B6" s="4">
-        <v>527</v>
+        <v>572</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" si="0"/>
-        <v>1.563473462485537E-2</v>
+        <v>1.5894186951205959E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1020,11 +1020,11 @@
         <v>7</v>
       </c>
       <c r="B7" s="4">
-        <v>1619</v>
+        <v>1704</v>
       </c>
       <c r="C7" s="12">
         <f t="shared" si="0"/>
-        <v>4.8031566143531018E-2</v>
+        <v>4.7349116372124044E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1032,11 +1032,11 @@
         <v>8</v>
       </c>
       <c r="B8" s="4">
-        <v>3671</v>
+        <v>3889</v>
       </c>
       <c r="C8" s="12">
         <f t="shared" si="0"/>
-        <v>0.1089091286676358</v>
+        <v>0.10806379904412582</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1044,11 +1044,11 @@
         <v>9</v>
       </c>
       <c r="B9" s="4">
-        <v>3051</v>
+        <v>3260</v>
       </c>
       <c r="C9" s="12">
         <f t="shared" si="0"/>
-        <v>9.0515323226629488E-2</v>
+        <v>9.0585750805824164E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1056,11 +1056,11 @@
         <v>10</v>
       </c>
       <c r="B10" s="4">
-        <v>3939</v>
+        <v>4196</v>
       </c>
       <c r="C10" s="12">
         <f t="shared" si="0"/>
-        <v>0.11685999940665144</v>
+        <v>0.11659442036234301</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1068,11 +1068,11 @@
         <v>11</v>
       </c>
       <c r="B11" s="4">
-        <v>4444</v>
+        <v>4746</v>
       </c>
       <c r="C11" s="12">
         <f t="shared" si="0"/>
-        <v>0.13184205061263238</v>
+        <v>0.13187729243081028</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1080,11 +1080,11 @@
         <v>12</v>
       </c>
       <c r="B12" s="4">
-        <v>4443</v>
+        <v>4761</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" si="0"/>
-        <v>0.13181238318450172</v>
+        <v>0.13229409803267755</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1092,11 +1092,11 @@
         <v>13</v>
       </c>
       <c r="B13" s="4">
-        <v>11808</v>
+        <v>12647</v>
       </c>
       <c r="C13" s="12">
         <f t="shared" si="0"/>
-        <v>0.3503129913667784</v>
+        <v>0.35142269645437368</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="B15" s="8">
         <f>SUM(B2:B14)</f>
-        <v>33707</v>
+        <v>35988</v>
       </c>
       <c r="C15" s="15">
         <f t="shared" si="0"/>
@@ -1133,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92BAF56-3443-4211-AC39-FD818DE6BEEB}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1155,11 +1155,11 @@
         <v>16</v>
       </c>
       <c r="B2" s="7">
-        <v>14249</v>
+        <v>15209</v>
       </c>
       <c r="C2" s="12">
         <f>B2/$B$5</f>
-        <v>0.42273118343370814</v>
+        <v>0.42261309325330665</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1167,11 +1167,11 @@
         <v>17</v>
       </c>
       <c r="B3" s="7">
-        <v>19457</v>
+        <v>20778</v>
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C5" si="0">B3/$B$5</f>
-        <v>0.57723914913816121</v>
+        <v>0.57735911970656884</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="C4" s="12">
         <f t="shared" si="0"/>
-        <v>2.9667428130655354E-5</v>
+        <v>2.7787040124485938E-5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B5" s="1">
         <f>SUM(B2:B4)</f>
-        <v>33707</v>
+        <v>35988</v>
       </c>
       <c r="C5" s="16">
         <f t="shared" si="0"/>
@@ -1209,7 +1209,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1233,11 +1233,11 @@
         <v>23</v>
       </c>
       <c r="B2" s="10">
-        <v>648</v>
+        <v>690</v>
       </c>
       <c r="C2" s="12">
         <f>B2/$B$8</f>
-        <v>1.9224493428664668E-2</v>
+        <v>1.9173057685895299E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1245,11 +1245,11 @@
         <v>21</v>
       </c>
       <c r="B3" s="9">
-        <v>3220</v>
+        <v>3413</v>
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C8" si="0">B3/$B$8</f>
-        <v>9.552911858071024E-2</v>
+        <v>9.4837167944870515E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1257,11 +1257,11 @@
         <v>22</v>
       </c>
       <c r="B4" s="10">
-        <v>16092</v>
+        <v>16964</v>
       </c>
       <c r="C4" s="12">
         <f t="shared" si="0"/>
-        <v>0.47740825347850596</v>
+        <v>0.4713793486717795</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1269,11 +1269,11 @@
         <v>25</v>
       </c>
       <c r="B5" s="10">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" si="0"/>
-        <v>5.3994719197792748E-3</v>
+        <v>5.3073246637768143E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1281,11 +1281,11 @@
         <v>20</v>
       </c>
       <c r="B6" s="4">
-        <v>13544</v>
+        <v>14709</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" si="0"/>
-        <v>0.40181564660159613</v>
+        <v>0.40871957319106367</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C7" s="12">
         <f t="shared" si="0"/>
-        <v>6.230159907437624E-4</v>
+        <v>5.8352784261420478E-4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1306,7 +1306,7 @@
       </c>
       <c r="B8" s="2">
         <f>SUM(B2:B7)</f>
-        <v>33707</v>
+        <v>35988</v>
       </c>
       <c r="C8" s="16">
         <f t="shared" si="0"/>

</xml_diff>